<commit_message>
PAS-6576 fixed updatedVinRenewal Test, left only 1 vehicle in it. Fixed typos in excel files, added AssignmentTab data to the yaml file for choice product to fill it properly during the test
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/UpdatedVIN_CA_SELECT.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/UpdatedVIN_CA_SELECT.xlsx
@@ -595,7 +595,7 @@
   <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,16 +819,16 @@
         <v>58</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="AG2" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="AI2">
         <v>20000101</v>
@@ -935,16 +935,16 @@
         <v>40</v>
       </c>
       <c r="AE3" s="4" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="AF3" s="4" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="AH3" s="4" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="AI3">
         <v>20010101</v>

</xml_diff>